<commit_message>
Updated excel with problems solved and cheats
</commit_message>
<xml_diff>
--- a/Blind 75 cheatsheet.xlsx
+++ b/Blind 75 cheatsheet.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GIT\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F58EBD-C9BF-471B-9D01-FC436781DAE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF56036-0ED5-447E-9A50-693234BC5126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blind 75" sheetId="1" r:id="rId1"/>
     <sheet name="TOP INterview Questions" sheetId="3" r:id="rId2"/>
     <sheet name="Algorithms" sheetId="2" r:id="rId3"/>
+    <sheet name="Interesting Questions" sheetId="4" r:id="rId4"/>
+    <sheet name="Problem Mnemonics" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="167">
   <si>
     <t>Domain</t>
   </si>
@@ -378,6 +380,221 @@
   </si>
   <si>
     <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/92/array/</t>
+  </si>
+  <si>
+    <t>Two pointer</t>
+  </si>
+  <si>
+    <t>LC 189. Rotate Array</t>
+  </si>
+  <si>
+    <t>The solution is to reverse 3 times. First is to reverse the entire array , then rotate till k and then the values after k. Rotaion code is a while loop with swapping in python</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/BHr381Guz3Y </t>
+  </si>
+  <si>
+    <t>Two Pointer/Linked List</t>
+  </si>
+  <si>
+    <t>19. Remove Nth Node From End of List</t>
+  </si>
+  <si>
+    <t>The 2 pointer solution involves creating a dummy head with left pointer and the right pointer 'n' steps further. Loop this until right is None and make left = left.next.next.
+There also exists a recursion method. Check the Discussion tab.</t>
+  </si>
+  <si>
+    <t>189. Rotate array</t>
+  </si>
+  <si>
+    <t>Given an array, rotate the array to the right by k steps, where k is non-negative.
+Reverse the entire array , then reverse from 0 to k , then k+1 to end</t>
+  </si>
+  <si>
+    <t>Sliding Window/Two pointer</t>
+  </si>
+  <si>
+    <t>567. Permutation in String</t>
+  </si>
+  <si>
+    <t>Medium/hard solution check out video</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.youtube.com/watch?v=UbyhOgBN834&amp;t=1s </t>
+  </si>
+  <si>
+    <t>BFS/DFS</t>
+  </si>
+  <si>
+    <t>116. Populating Next Right Pointers in Each Node</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/U4hFQCa1Cq0 </t>
+  </si>
+  <si>
+    <t>you only need one pointer to the left most node of a layer, others must be connectedone layer above through the next. Rest all can be traversed. Check solution for full understanding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BFS/Dynamic </t>
+  </si>
+  <si>
+    <t>542. 01 Matrix</t>
+  </si>
+  <si>
+    <t>BFS - Iterates through array, keeps zeros  unchanges, makes rest as inf and add nodes to queue. Pop queue add 1 to neighbors distance accordingy.
+Dyanmic - Iterate once from left and down setting minimum values. And secon time from right to up. Check submission</t>
+  </si>
+  <si>
+    <t>BFS</t>
+  </si>
+  <si>
+    <t>994. Rotting Oranges</t>
+  </si>
+  <si>
+    <t>Uses multisource BFS to traverse and convert frsh to rotten. Check video for details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.youtube.com/watch?v=y704fEOx0s0&amp;t=1s </t>
+  </si>
+  <si>
+    <t>Can be solved iteratively(optimal) and recursion. For iterative, start with 2 pointers and a temp varaible. Think the soulution is intuitive. Recursion is abrain turner, plot it and understand. Check the video</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/G0_I-ZF0S38 </t>
+  </si>
+  <si>
+    <t>77. Combinations</t>
+  </si>
+  <si>
+    <t>Backtracking/Recursion</t>
+  </si>
+  <si>
+    <t>Complex backtracking. Watch video</t>
+  </si>
+  <si>
+    <t>Problem Category</t>
+  </si>
+  <si>
+    <t>All backtracking problems, require to build a tree type iteration, the function remains the same just operation changes with task</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/permutations/discuss/18284/Backtrack-Summary%3A-General-Solution-for-10-Questions!!!!!!!!-Python-(Combination-Sum-Subsets-Permutation-Palindrome) </t>
+  </si>
+  <si>
+    <t>46. Permutations</t>
+  </si>
+  <si>
+    <t>Use the backtracking "problem mnemonics"</t>
+  </si>
+  <si>
+    <t>Can be solved in Top down approach (recursion+memoization) or bottom up aproach (Dynamic Prog). Top down is straight forward, plot graph and its understandable. DP solution is fibonnaci series and try to do it using no array and only 2 variables.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Good problem. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The max amount at a instance i can be the max(num[i] + summ till (i-2) or sum till i-1</t>
+    </r>
+  </si>
+  <si>
+    <t>Bit manipulation</t>
+  </si>
+  <si>
+    <t>231. Power of Two</t>
+  </si>
+  <si>
+    <t>Detailed bit description - https://leetcode.com/problems/power-of-two/discuss/1638707/PythonC%2B%2BJava-Detailly-Explain-Why-n-and-n-1-Works-oror-1-Line-oror-100-Faster-oror-Easy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can be done iteratively or smart bit manipulation. Iteratively - modulo n (gets the last bit) add it to count and shift number by one to right.
+For bit manipulation go on n&amp;(n-1) until n ==0, and increment count. This works </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Good problem. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Iterate with I from 0-31, right shift number by i and &amp; with 1. This extracts the bit in units place. Now place this bit in 31st place of a new number. This done by orring 0 with the bit left shifted 31-i places</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Identify Optimal Solution from Constraints </t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Max Complexity</t>
+  </si>
+  <si>
+    <t>10^18</t>
+  </si>
+  <si>
+    <t>10^4</t>
+  </si>
+  <si>
+    <t>10^8</t>
+  </si>
+  <si>
+    <t>O(N)</t>
+  </si>
+  <si>
+    <t>O(logN)</t>
+  </si>
+  <si>
+    <t>O(N^2)</t>
+  </si>
+  <si>
+    <t>10^6</t>
+  </si>
+  <si>
+    <t>O(Nlog(N))</t>
+  </si>
+  <si>
+    <t>N^3</t>
+  </si>
+  <si>
+    <t>85-90</t>
+  </si>
+  <si>
+    <t>O(N^4)</t>
+  </si>
+  <si>
+    <t>O(2^N)</t>
+  </si>
+  <si>
+    <t>N!</t>
   </si>
 </sst>
 </file>
@@ -530,7 +747,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -602,6 +819,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -886,9 +1115,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1073,17 +1302,19 @@
       </c>
       <c r="D12" s="24"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="24"/>
+      <c r="D13" s="29" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
@@ -1116,10 +1347,12 @@
       <c r="B16" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="24"/>
+      <c r="D16" s="24" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
@@ -1128,10 +1361,12 @@
       <c r="B17" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="24"/>
+      <c r="D17" s="24" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
@@ -1200,10 +1435,12 @@
       <c r="B23" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="24"/>
+      <c r="D23" s="24" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
@@ -1313,7 +1550,7 @@
       </c>
       <c r="D32" s="24"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -1325,7 +1562,7 @@
       </c>
       <c r="D33" s="24"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -1337,7 +1574,7 @@
       </c>
       <c r="D34" s="24"/>
     </row>
-    <row r="35" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -1349,7 +1586,7 @@
       </c>
       <c r="D35" s="24"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -1361,7 +1598,7 @@
       </c>
       <c r="D36" s="24"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -1373,7 +1610,7 @@
       </c>
       <c r="D37" s="24"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -1385,7 +1622,7 @@
       </c>
       <c r="D38" s="24"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -1397,7 +1634,7 @@
       </c>
       <c r="D39" s="24"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -1409,19 +1646,24 @@
       </c>
       <c r="D40" s="24"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>40</v>
       </c>
       <c r="B41" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D41" s="24"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D41" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="E41" s="19" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -1433,7 +1675,7 @@
       </c>
       <c r="D42" s="24"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -1445,7 +1687,7 @@
       </c>
       <c r="D43" s="24"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -1457,7 +1699,7 @@
       </c>
       <c r="D44" s="24"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -1469,7 +1711,7 @@
       </c>
       <c r="D45" s="24"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -1481,7 +1723,7 @@
       </c>
       <c r="D46" s="24"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -1493,7 +1735,7 @@
       </c>
       <c r="D47" s="24"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -1933,9 +2175,10 @@
     <hyperlink ref="C77" r:id="rId76" display="https://leetcode.com/problems/find-median-from-data-stream/" xr:uid="{57CFF2A3-7378-4CF7-8A79-CDA750EBBBD6}"/>
     <hyperlink ref="E5" r:id="rId77" xr:uid="{2CB97602-D527-4D56-8340-AFF1BA3A7404}"/>
     <hyperlink ref="E7" r:id="rId78" xr:uid="{DC6C85AD-4976-4301-A6DB-19DE7BC67D1E}"/>
+    <hyperlink ref="E41" r:id="rId79" xr:uid="{DC55541E-51CF-4028-B660-9D4B0F68E90E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId79"/>
+  <pageSetup orientation="portrait" r:id="rId80"/>
 </worksheet>
 </file>
 
@@ -1966,7 +2209,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2012,4 +2255,333 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C33D644C-0702-4680-A647-3F23A1C17400}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="49.5546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="32.33203125" style="27" customWidth="1"/>
+    <col min="5" max="5" width="32.33203125" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{508F3E18-DC81-439A-90BD-BE33034915B7}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{84C2B14F-8230-4724-B416-F222516D4BF6}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{F9E75F9B-11CD-4C5B-915D-2DC84AE203D1}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{085CA4B8-C036-44F7-9DDB-95783FFC4FA8}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{125CBD72-80F0-45E7-9C78-47683AA1F5DE}"/>
+    <hyperlink ref="E5" r:id="rId6" xr:uid="{A6AE1D5B-961F-4CF3-B2DD-469B5CB0EE75}"/>
+    <hyperlink ref="C6" r:id="rId7" xr:uid="{C4A35233-2ABA-4E0F-B0FF-99999FCE39F7}"/>
+    <hyperlink ref="E6" r:id="rId8" xr:uid="{BAEF9715-1B3D-41AF-9D00-A4AE4669FA03}"/>
+    <hyperlink ref="C7" r:id="rId9" xr:uid="{1EB4CEF5-9394-4059-885F-59A37886C136}"/>
+    <hyperlink ref="C8" r:id="rId10" xr:uid="{E6DCEF1D-3B95-41C7-99B6-B96235FD5A67}"/>
+    <hyperlink ref="E8" r:id="rId11" xr:uid="{64A7E8A5-C174-4CBA-85D9-B9EC802344EA}"/>
+    <hyperlink ref="C9" r:id="rId12" xr:uid="{375FA4AF-5531-41AC-B5A3-F1286E748366}"/>
+    <hyperlink ref="C10" r:id="rId13" xr:uid="{5C8C17CF-FF27-44EF-9F7D-5697E279767F}"/>
+    <hyperlink ref="C11" r:id="rId14" xr:uid="{A509631F-AAC7-443C-B840-A737F2A0F22D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E2E9C92-4073-4ED7-AA15-F248F8C57B6A}">
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="3" width="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>500</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>20</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>11</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{FBC2CEF9-BEC4-4A67-9632-B5DF9D48C0BB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>